<commit_message>
add explanation to understand the error : loss, lesate square (moindre carre)
</commit_message>
<xml_diff>
--- a/REGRESSION.xlsx
+++ b/REGRESSION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mizab\OneDrive\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A1775A-1AE6-4C03-815C-8E23A6AA292A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C1F43E-8C42-4D84-86BB-BA147516BBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,9 @@
     <sheet name="PRACTICE 3" sheetId="3" r:id="rId3"/>
     <sheet name="PRACTICAL4" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PRACTICAL4!$L$39:$P$54</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Study Hours (X)</t>
   </si>
@@ -108,6 +133,30 @@
   <si>
     <t>Prix (en 1000€)</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>LINEST</t>
+  </si>
+  <si>
+    <t>ESTIMATION</t>
+  </si>
+  <si>
+    <t>USING MATRIX</t>
+  </si>
+  <si>
+    <t>LINEARE</t>
+  </si>
+  <si>
+    <t>SLOP</t>
+  </si>
+  <si>
+    <t>DISTANCE</t>
+  </si>
 </sst>
 </file>
 
@@ -115,7 +164,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -165,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,8 +233,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -208,12 +269,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -233,6 +318,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -242,18 +333,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -3030,8 +3142,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3970,6 +4083,426 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LINEARE</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> REGRESSION</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>PRACTICAL4!$M$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>PRACTICAL4!$L$40:$L$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>PRACTICAL4!$M$40:$M$47</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.0_);_("$"* \(#,##0.0\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-41D7-4F75-B734-A3A386542612}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="342621584"/>
+        <c:axId val="342622416"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="342621584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="342622416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="342622416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="342621584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4250,6 +4783,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="229">
   <cs:axisTitle>
@@ -7401,6 +7974,522 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8185,6 +9274,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05DAF630-AF63-4862-967A-503ECEC8A010}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8513,61 +9638,61 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8583,7 +9708,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8674,10 +9799,10 @@
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="9"/>
+      <c r="D25" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8765,10 +9890,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E226707-C9D7-4195-A30B-AA04FC29F583}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+    <sheetView tabSelected="1" topLeftCell="J33" workbookViewId="0">
+      <selection activeCell="T53" sqref="T53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8778,1029 +9903,1272 @@
     <col min="4" max="4" width="19.88671875" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="9">
         <v>80</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="9">
         <v>3</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="9">
         <v>10</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="9">
         <v>3.2</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="10">
         <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="9">
         <v>120</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>4</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="9">
         <v>5</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>2.5</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="10">
         <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <v>60</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="9">
         <v>2</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>15</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>8.6999999999999993</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="10">
         <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="9">
         <v>100</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>4</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="9">
         <v>20</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>5</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="10">
         <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>90</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>3</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>7</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>4.3</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="10">
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>150</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <v>5</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>3</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>1</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="10">
         <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="9">
         <v>200</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="9">
         <v>6</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="9">
         <v>1</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="9">
         <v>0.8</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="10">
         <v>410</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="9">
         <v>75</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="9">
         <v>3</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="9">
         <v>25</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="9">
         <v>10</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="10">
         <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="9">
         <v>110</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="9">
         <v>4</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="9">
         <v>30</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="9">
         <v>7.5</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="10">
         <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="9">
         <v>55</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="9">
         <v>2</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="9">
         <v>40</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="9">
         <v>15</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="10">
         <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="9">
         <v>130</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="9">
         <v>5</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="9">
         <v>5</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="9">
         <v>3</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="10">
         <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="9">
         <v>95</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="9">
         <v>3</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="9">
         <v>18</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="9">
         <v>4</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="10">
         <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="9">
         <v>160</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="9">
         <v>5</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="9">
         <v>2</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="9">
         <v>2</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="10">
         <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="12">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="9">
         <v>180</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="9">
         <v>6</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="9">
         <v>0</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="9">
         <v>1.2</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="10">
         <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="12">
+      <c r="A16" s="9">
         <v>15</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="9">
         <v>60</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="9">
         <v>2</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="9">
         <v>10</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="9">
         <v>12</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="10">
         <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="9">
         <v>85</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="9">
         <v>3</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="9">
         <v>12</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="9">
         <v>9.5</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="10">
         <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="12">
+      <c r="A18" s="9">
         <v>17</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="9">
         <v>140</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="9">
         <v>4</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="9">
         <v>4</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="9">
         <v>3</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="10">
         <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="12">
+      <c r="A19" s="9">
         <v>18</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="9">
         <v>170</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="9">
         <v>5</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="9">
         <v>6</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="9">
         <v>2.5</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="10">
         <v>360</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="12">
+      <c r="A20" s="9">
         <v>19</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="9">
         <v>75</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="9">
         <v>2</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="9">
         <v>30</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="9">
         <v>13</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="10">
         <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="12">
+      <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="9">
         <v>105</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="9">
         <v>4</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="9">
         <v>20</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="9">
         <v>7</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="10">
         <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="12">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="9">
         <v>65</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="9">
         <v>2</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="9">
         <v>35</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="9">
         <v>14</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="10">
         <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="12">
+      <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="9">
         <v>90</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="9">
         <v>3</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="9">
         <v>22</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="9">
         <v>6</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="10">
         <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="12">
+      <c r="A24" s="9">
         <v>23</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="9">
         <v>125</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="9">
         <v>5</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="9">
         <v>8</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="10">
         <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="12">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="9">
         <v>135</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="9">
         <v>4</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="9">
         <v>3</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="9">
         <v>1.5</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="10">
         <v>300</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="12">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="9">
         <v>150</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="9">
         <v>5</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="9">
         <v>1</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="9">
         <v>1</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="10">
         <v>325</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="12">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="9">
         <v>95</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="9">
         <v>3</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="9">
         <v>17</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="9">
         <v>4.7</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="10">
         <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="12">
+      <c r="A28" s="9">
         <v>27</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="9">
         <v>160</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="9">
         <v>5</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="9">
         <v>0</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="9">
         <v>0.5</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="10">
         <v>345</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="12">
+      <c r="A29" s="9">
         <v>28</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="9">
         <v>175</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="9">
         <v>6</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="9">
         <v>2</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="10">
         <v>380</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="12">
+      <c r="A30" s="9">
         <v>29</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="9">
         <v>70</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="9">
         <v>2</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="9">
         <v>28</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="9">
         <v>11</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="10">
         <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="12">
+      <c r="A31" s="9">
         <v>30</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="9">
         <v>100</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="9">
         <v>4</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="9">
         <v>19</v>
       </c>
-      <c r="E31" s="12">
+      <c r="E31" s="9">
         <v>6.5</v>
       </c>
-      <c r="F31" s="13">
+      <c r="F31" s="10">
         <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="12">
+      <c r="A32" s="9">
         <v>31</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="9">
         <v>60</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="9">
         <v>2</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="9">
         <v>38</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="9">
         <v>16</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="10">
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="12">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" s="9">
         <v>32</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="9">
         <v>85</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="9">
         <v>3</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="9">
         <v>21</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="9">
         <v>8</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="10">
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="12">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" s="9">
         <v>33</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="9">
         <v>145</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="9">
         <v>5</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="9">
         <v>4</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="9">
         <v>2</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="10">
         <v>315</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="12">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" s="9">
         <v>34</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="9">
         <v>165</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="9">
         <v>6</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="9">
         <v>2</v>
       </c>
-      <c r="E35" s="12">
+      <c r="E35" s="9">
         <v>1.3</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F35" s="10">
         <v>355</v>
       </c>
+      <c r="N35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q35" s="13"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="12">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" s="9">
         <v>35</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="9">
         <v>78</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="9">
         <v>2</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="9">
         <v>27</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="9">
         <v>12.5</v>
       </c>
-      <c r="F36" s="13">
+      <c r="F36" s="10">
         <v>155</v>
       </c>
+      <c r="N36" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="O36" s="16"/>
+      <c r="P36" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="12">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" s="9">
         <v>36</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="9">
         <v>98</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="9">
         <v>3</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D37" s="9">
         <v>15</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="9">
         <v>5.5</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="10">
         <v>200</v>
       </c>
+      <c r="N37" s="15" cm="1">
+        <f t="array" ref="N37:O37">LINEST(M40:M47,L40:L47,TRUE)</f>
+        <v>-14.77985230597743</v>
+      </c>
+      <c r="O37" s="15">
+        <v>342.46446983419258</v>
+      </c>
+      <c r="P37">
+        <f>SLOPE(M40:M47,L40:L47)</f>
+        <v>-14.77985230597743</v>
+      </c>
+      <c r="Q37">
+        <f>INTERCEPT(M40:M47,L40:L47)</f>
+        <v>342.46446983419258</v>
+      </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="12">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" s="9">
         <v>37</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="9">
         <v>132</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="9">
         <v>5</v>
       </c>
-      <c r="D38" s="12">
+      <c r="D38" s="9">
         <v>6</v>
       </c>
-      <c r="E38" s="12">
+      <c r="E38" s="9">
         <v>3</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F38" s="10">
         <v>295</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="12">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A39" s="9">
         <v>38</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B39" s="9">
         <v>182</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="9">
         <v>6</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39" s="9">
         <v>1</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E39" s="9">
         <v>0.7</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F39" s="10">
         <v>400</v>
       </c>
+      <c r="L39" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O39" s="23" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="12">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A40" s="9">
         <v>39</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40" s="9">
         <v>58</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C40" s="9">
         <v>2</v>
       </c>
-      <c r="D40" s="12">
+      <c r="D40" s="9">
         <v>41</v>
       </c>
-      <c r="E40" s="12">
+      <c r="E40" s="9">
         <v>18</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F40" s="10">
         <v>110</v>
       </c>
+      <c r="L40" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="M40" s="20">
+        <v>155</v>
+      </c>
+      <c r="N40" s="21">
+        <f>$N$37*L40+$O$37</f>
+        <v>157.7163160094747</v>
+      </c>
+      <c r="O40" s="24">
+        <f>N40-M40</f>
+        <v>2.7163160094746956</v>
+      </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="12">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A41" s="9">
         <v>40</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="9">
         <v>88</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41" s="9">
         <v>3</v>
       </c>
-      <c r="D41" s="12">
+      <c r="D41" s="9">
         <v>20</v>
       </c>
-      <c r="E41" s="12">
+      <c r="E41" s="9">
         <v>10</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F41" s="10">
         <v>175</v>
       </c>
+      <c r="L41" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="M41" s="20">
+        <v>200</v>
+      </c>
+      <c r="N41" s="21">
+        <f>$N$37*L41+$O$37</f>
+        <v>261.17528215131671</v>
+      </c>
+      <c r="O41" s="24">
+        <f t="shared" ref="O41:O47" si="0">N41-M41</f>
+        <v>61.175282151316708</v>
+      </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="12">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A42" s="9">
         <v>41</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42" s="9">
         <v>115</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="9">
         <v>4</v>
       </c>
-      <c r="D42" s="12">
+      <c r="D42" s="9">
         <v>7</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E42" s="9">
         <v>4</v>
       </c>
-      <c r="F42" s="13">
+      <c r="F42" s="10">
         <v>260</v>
       </c>
+      <c r="L42" s="9">
+        <v>3</v>
+      </c>
+      <c r="M42" s="20">
+        <v>295</v>
+      </c>
+      <c r="N42" s="21">
+        <f>$N$37*L42+$O$37</f>
+        <v>298.12491291626031</v>
+      </c>
+      <c r="O42" s="24">
+        <f t="shared" si="0"/>
+        <v>3.124912916260314</v>
+      </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="12">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" s="9">
         <v>42</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B43" s="9">
         <v>148</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="9">
         <v>5</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43" s="9">
         <v>3</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E43" s="9">
         <v>2.1</v>
       </c>
-      <c r="F43" s="13">
+      <c r="F43" s="10">
         <v>320</v>
       </c>
+      <c r="L43" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="M43" s="20">
+        <v>400</v>
+      </c>
+      <c r="N43" s="21">
+        <f>$N$37*L43+$O$37</f>
+        <v>332.11857322000839</v>
+      </c>
+      <c r="O43" s="25">
+        <f>N43-M43</f>
+        <v>-67.881426779991614</v>
+      </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="12">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" s="9">
         <v>43</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44" s="9">
         <v>90</v>
       </c>
-      <c r="C44" s="12">
+      <c r="C44" s="9">
         <v>3</v>
       </c>
-      <c r="D44" s="12">
+      <c r="D44" s="9">
         <v>25</v>
       </c>
-      <c r="E44" s="12">
+      <c r="E44" s="9">
         <v>7</v>
       </c>
-      <c r="F44" s="13">
+      <c r="F44" s="10">
         <v>185</v>
       </c>
+      <c r="L44" s="9">
+        <v>18</v>
+      </c>
+      <c r="M44" s="20">
+        <v>110</v>
+      </c>
+      <c r="N44" s="21">
+        <f>$N$37*L44+$O$37</f>
+        <v>76.427128326598847</v>
+      </c>
+      <c r="O44" s="24">
+        <f t="shared" si="0"/>
+        <v>-33.572871673401153</v>
+      </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="12">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45" s="9">
         <v>44</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B45" s="9">
         <v>168</v>
       </c>
-      <c r="C45" s="12">
+      <c r="C45" s="9">
         <v>6</v>
       </c>
-      <c r="D45" s="12">
+      <c r="D45" s="9">
         <v>2</v>
       </c>
-      <c r="E45" s="12">
+      <c r="E45" s="9">
         <v>1</v>
       </c>
-      <c r="F45" s="13">
+      <c r="F45" s="10">
         <v>370</v>
       </c>
+      <c r="L45" s="9">
+        <v>10</v>
+      </c>
+      <c r="M45" s="20">
+        <v>175</v>
+      </c>
+      <c r="N45" s="21">
+        <f>$N$37*L45+$O$37</f>
+        <v>194.66594677441827</v>
+      </c>
+      <c r="O45" s="24">
+        <f t="shared" si="0"/>
+        <v>19.665946774418273</v>
+      </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="12">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46" s="9">
         <v>45</v>
       </c>
-      <c r="B46" s="12">
+      <c r="B46" s="9">
         <v>72</v>
       </c>
-      <c r="C46" s="12">
+      <c r="C46" s="9">
         <v>2</v>
       </c>
-      <c r="D46" s="12">
+      <c r="D46" s="9">
         <v>30</v>
       </c>
-      <c r="E46" s="12">
+      <c r="E46" s="9">
         <v>13.5</v>
       </c>
-      <c r="F46" s="13">
+      <c r="F46" s="10">
         <v>140</v>
       </c>
+      <c r="L46" s="9">
+        <v>4</v>
+      </c>
+      <c r="M46" s="20">
+        <v>260</v>
+      </c>
+      <c r="N46" s="21">
+        <f>$N$37*L46+$O$37</f>
+        <v>283.34506061028287</v>
+      </c>
+      <c r="O46" s="24">
+        <f t="shared" si="0"/>
+        <v>23.345060610282871</v>
+      </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="12">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47" s="9">
         <v>46</v>
       </c>
-      <c r="B47" s="12">
+      <c r="B47" s="9">
         <v>107</v>
       </c>
-      <c r="C47" s="12">
+      <c r="C47" s="9">
         <v>4</v>
       </c>
-      <c r="D47" s="12">
+      <c r="D47" s="9">
         <v>17</v>
       </c>
-      <c r="E47" s="12">
+      <c r="E47" s="9">
         <v>5.5</v>
       </c>
-      <c r="F47" s="13">
+      <c r="F47" s="10">
         <v>225</v>
       </c>
+      <c r="L47" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="M47" s="20">
+        <v>320</v>
+      </c>
+      <c r="N47" s="21">
+        <f>$N$37*L47+$O$37</f>
+        <v>311.42677999163999</v>
+      </c>
+      <c r="O47" s="24">
+        <f t="shared" si="0"/>
+        <v>-8.5732200083600105</v>
+      </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="12">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" s="9">
         <v>47</v>
       </c>
-      <c r="B48" s="12">
+      <c r="B48" s="9">
         <v>59</v>
       </c>
-      <c r="C48" s="12">
+      <c r="C48" s="9">
         <v>2</v>
       </c>
-      <c r="D48" s="12">
+      <c r="D48" s="9">
         <v>39</v>
       </c>
-      <c r="E48" s="12">
+      <c r="E48" s="9">
         <v>17</v>
       </c>
-      <c r="F48" s="13">
+      <c r="F48" s="10">
         <v>105</v>
       </c>
+      <c r="L48" s="18">
+        <v>2</v>
+      </c>
+      <c r="M48" s="19"/>
+      <c r="N48" s="21">
+        <f>$N$37*L48+$O$37</f>
+        <v>312.9047652222377</v>
+      </c>
+      <c r="O48" s="24"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="12">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" s="9">
         <v>48</v>
       </c>
-      <c r="B49" s="12">
+      <c r="B49" s="9">
         <v>83</v>
       </c>
-      <c r="C49" s="12">
+      <c r="C49" s="9">
         <v>3</v>
       </c>
-      <c r="D49" s="12">
+      <c r="D49" s="9">
         <v>23</v>
       </c>
-      <c r="E49" s="12">
+      <c r="E49" s="9">
         <v>9</v>
       </c>
-      <c r="F49" s="13">
+      <c r="F49" s="10">
         <v>170</v>
       </c>
+      <c r="L49" s="18">
+        <v>3.2</v>
+      </c>
+      <c r="M49" s="19"/>
+      <c r="N49" s="21">
+        <f>$N$37*L49+$O$37</f>
+        <v>295.16894245506478</v>
+      </c>
+      <c r="O49" s="24"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="12">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" s="9">
         <v>49</v>
       </c>
-      <c r="B50" s="12">
+      <c r="B50" s="9">
         <v>137</v>
       </c>
-      <c r="C50" s="12">
+      <c r="C50" s="9">
         <v>5</v>
       </c>
-      <c r="D50" s="12">
+      <c r="D50" s="9">
         <v>5</v>
       </c>
-      <c r="E50" s="12">
+      <c r="E50" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F50" s="13">
+      <c r="F50" s="10">
         <v>305</v>
       </c>
+      <c r="L50" s="18">
+        <v>6</v>
+      </c>
+      <c r="N50" s="21">
+        <f>$N$37*L50+$O$37</f>
+        <v>253.78535599832799</v>
+      </c>
+      <c r="O50" s="24"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="12">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51" s="9">
         <v>50</v>
       </c>
-      <c r="B51" s="12">
+      <c r="B51" s="9">
         <v>158</v>
       </c>
-      <c r="C51" s="12">
+      <c r="C51" s="9">
         <v>5</v>
       </c>
-      <c r="D51" s="12">
+      <c r="D51" s="9">
         <v>2</v>
       </c>
-      <c r="E51" s="12">
+      <c r="E51" s="9">
         <v>1.3</v>
       </c>
-      <c r="F51" s="13">
+      <c r="F51" s="10">
         <v>335</v>
       </c>
+      <c r="L51" s="18">
+        <v>7</v>
+      </c>
+      <c r="N51" s="21">
+        <f>$N$37*L51+$O$37</f>
+        <v>239.00550369235057</v>
+      </c>
+      <c r="O51" s="24"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L52" s="18">
+        <v>8</v>
+      </c>
+      <c r="N52" s="21">
+        <f>$N$37*L52+$O$37</f>
+        <v>224.22565138637316</v>
+      </c>
+      <c r="O52" s="24"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L53" s="18">
+        <v>7.5</v>
+      </c>
+      <c r="N53" s="21">
+        <f>$N$37*L53+$O$37</f>
+        <v>231.61557753936188</v>
+      </c>
+      <c r="O53" s="24"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L54" s="18">
+        <v>3.4</v>
+      </c>
+      <c r="M54" s="19"/>
+      <c r="N54" s="21">
+        <f>$N$37*L54+$O$37</f>
+        <v>292.2129719938693</v>
+      </c>
+      <c r="O54" s="24"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L55" s="17">
+        <v>3.2</v>
+      </c>
+      <c r="N55" s="22">
+        <f>$N$37*L55+$O$37</f>
+        <v>295.16894245506478</v>
+      </c>
+      <c r="O55" s="24"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="P35:Q35"/>
+  </mergeCells>
+  <conditionalFormatting sqref="O40:O47">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>-3.35</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>